<commit_message>
Dodane vse meje in barvanja
</commit_message>
<xml_diff>
--- a/Meje za meritve.xlsx
+++ b/Meje za meritve.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26529"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasak\ProjektAljaz\Avtomatiziranje-elektro-zapiskov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACC08278-E2E0-4F3D-8910-1494EF23EE5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1067D2-6D34-41F1-B8FE-2109CDC08CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15796" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-83" yWindow="0" windowWidth="14566" windowHeight="15563" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gG" sheetId="2" r:id="rId1"/>
     <sheet name="BCD" sheetId="3" r:id="rId2"/>
     <sheet name="NV" sheetId="4" r:id="rId3"/>
+    <sheet name="ZLOOP" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
   <si>
     <t>Nazivni tok nadtokovne zaščite</t>
   </si>
@@ -134,6 +135,572 @@
       </rPr>
       <t>PE</t>
     </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">1
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Najvišja impedanca napajalnega vira do zaščitne naprave</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>Najmanjši prerez</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">3
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Najvišja nazivna zmogljivost ali nastavitev zaščitne naprave
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">4
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Odklopni čas varovalke
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>5 s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Odklopni čas varovalk
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>0,4 s</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">6
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Miniaturni odklopnik
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">e      tipa B
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">5 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">× </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">7
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Miniaturni odklopnik tipa C
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">10 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">× </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">8
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Miniaturni odklopnik tipa D
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">= </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">20 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">× </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">9
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">Nastavljiv odklopnik
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">= 8 </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve">× </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <vertAlign val="superscript"/>
+        <sz val="9"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>I</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="6"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>N</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1,5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>2,5</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4,0</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="9"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>6,0</t>
+    </r>
+  </si>
+  <si>
+    <t>25/16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35/16 </t>
+  </si>
+  <si>
+    <t>50/25</t>
+  </si>
+  <si>
+    <t>70/35</t>
+  </si>
+  <si>
+    <t>95/50</t>
+  </si>
+  <si>
+    <t>120/70</t>
+  </si>
+  <si>
+    <t>X</t>
   </si>
 </sst>
 </file>
@@ -144,7 +711,7 @@
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
-  <fonts count="15" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -239,6 +806,44 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <b/>
+      <i/>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="6"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <b/>
+      <vertAlign val="superscript"/>
+      <sz val="9"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="8">
     <fill>
@@ -284,7 +889,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -652,11 +1257,39 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="94">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -924,6 +1557,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -940,6 +1594,69 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:oneCellAnchor>
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5759450" cy="9525"/>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Shape 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{08B1AE72-5487-40ED-8EC5-253C529C14C9}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="0"/>
+          <a:ext cx="5759450" cy="9525"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path w="5759450" h="9525">
+              <a:moveTo>
+                <a:pt x="5759195" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="0"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="0" y="9143"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="5759195" y="9143"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="5759195" y="0"/>
+              </a:lnTo>
+              <a:close/>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:solidFill>
+          <a:srgbClr val="000000"/>
+        </a:solidFill>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:oneCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1207,8 +1924,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19B6F0FC-680A-40AD-A774-83D15BC62DA5}">
   <dimension ref="A1:L34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N28" sqref="N28"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:L34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -2936,7 +3653,7 @@
   <dimension ref="A1:C33"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -3335,4 +4052,397 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4FE9D0-D252-4B66-A7CF-69234516F26F}">
+  <dimension ref="A1:I13"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:9" ht="106.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="94" t="s">
+        <v>28</v>
+      </c>
+      <c r="B1" s="94" t="s">
+        <v>29</v>
+      </c>
+      <c r="C1" s="94" t="s">
+        <v>30</v>
+      </c>
+      <c r="D1" s="94" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="94" t="s">
+        <v>32</v>
+      </c>
+      <c r="F1" s="94" t="s">
+        <v>33</v>
+      </c>
+      <c r="G1" s="94" t="s">
+        <v>34</v>
+      </c>
+      <c r="H1" s="94" t="s">
+        <v>35</v>
+      </c>
+      <c r="I1" s="95" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A2" s="97">
+        <v>500</v>
+      </c>
+      <c r="B2" s="96" t="s">
+        <v>37</v>
+      </c>
+      <c r="C2" s="97">
+        <v>16</v>
+      </c>
+      <c r="D2" s="97">
+        <v>97</v>
+      </c>
+      <c r="E2" s="97">
+        <v>53</v>
+      </c>
+      <c r="F2" s="97">
+        <v>76</v>
+      </c>
+      <c r="G2" s="97">
+        <v>30</v>
+      </c>
+      <c r="H2" s="97">
+        <v>7</v>
+      </c>
+      <c r="I2" s="98">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A3" s="97">
+        <v>500</v>
+      </c>
+      <c r="B3" s="96" t="s">
+        <v>38</v>
+      </c>
+      <c r="C3" s="97">
+        <v>20</v>
+      </c>
+      <c r="D3" s="97">
+        <v>115</v>
+      </c>
+      <c r="E3" s="97">
+        <v>57</v>
+      </c>
+      <c r="F3" s="97">
+        <v>94</v>
+      </c>
+      <c r="G3" s="97">
+        <v>34</v>
+      </c>
+      <c r="H3" s="97">
+        <v>3</v>
+      </c>
+      <c r="I3" s="98">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A4" s="97">
+        <v>500</v>
+      </c>
+      <c r="B4" s="96" t="s">
+        <v>39</v>
+      </c>
+      <c r="C4" s="97">
+        <v>25</v>
+      </c>
+      <c r="D4" s="97">
+        <v>135</v>
+      </c>
+      <c r="E4" s="97">
+        <v>66</v>
+      </c>
+      <c r="F4" s="97">
+        <v>114</v>
+      </c>
+      <c r="G4" s="97">
+        <v>35</v>
+      </c>
+      <c r="H4" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I4" s="98">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A5" s="97">
+        <v>400</v>
+      </c>
+      <c r="B5" s="96" t="s">
+        <v>40</v>
+      </c>
+      <c r="C5" s="97">
+        <v>32</v>
+      </c>
+      <c r="D5" s="97">
+        <v>145</v>
+      </c>
+      <c r="E5" s="97">
+        <v>59</v>
+      </c>
+      <c r="F5" s="97">
+        <v>133</v>
+      </c>
+      <c r="G5" s="97">
+        <v>40</v>
+      </c>
+      <c r="H5" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I5" s="98">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A6" s="97">
+        <v>300</v>
+      </c>
+      <c r="B6" s="97">
+        <v>10</v>
+      </c>
+      <c r="C6" s="97">
+        <v>50</v>
+      </c>
+      <c r="D6" s="97">
+        <v>125</v>
+      </c>
+      <c r="E6" s="97">
+        <v>41</v>
+      </c>
+      <c r="F6" s="97">
+        <v>132</v>
+      </c>
+      <c r="G6" s="97">
+        <v>33</v>
+      </c>
+      <c r="H6" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I6" s="98">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A7" s="97">
+        <v>200</v>
+      </c>
+      <c r="B7" s="97">
+        <v>16</v>
+      </c>
+      <c r="C7" s="97">
+        <v>63</v>
+      </c>
+      <c r="D7" s="97">
+        <v>175</v>
+      </c>
+      <c r="E7" s="97">
+        <v>73</v>
+      </c>
+      <c r="F7" s="97">
+        <v>179</v>
+      </c>
+      <c r="G7" s="97">
+        <v>55</v>
+      </c>
+      <c r="H7" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I7" s="98">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A8" s="97">
+        <v>200</v>
+      </c>
+      <c r="B8" s="99" t="s">
+        <v>41</v>
+      </c>
+      <c r="C8" s="97">
+        <v>80</v>
+      </c>
+      <c r="D8" s="97">
+        <v>133</v>
+      </c>
+      <c r="E8" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="F8" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="G8" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="H8" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I8" s="98">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A9" s="97">
+        <v>100</v>
+      </c>
+      <c r="B9" s="99" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9" s="97">
+        <v>100</v>
+      </c>
+      <c r="D9" s="97">
+        <v>136</v>
+      </c>
+      <c r="E9" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="G9" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="H9" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I9" s="98">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A10" s="97">
+        <v>100</v>
+      </c>
+      <c r="B10" s="99" t="s">
+        <v>43</v>
+      </c>
+      <c r="C10" s="97">
+        <v>125</v>
+      </c>
+      <c r="D10" s="97">
+        <v>141</v>
+      </c>
+      <c r="E10" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="G10" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I10" s="98">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A11" s="97">
+        <v>100</v>
+      </c>
+      <c r="B11" s="99" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="97">
+        <v>160</v>
+      </c>
+      <c r="D11" s="97">
+        <v>138</v>
+      </c>
+      <c r="E11" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="G11" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I11" s="98">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A12" s="97">
+        <v>50</v>
+      </c>
+      <c r="B12" s="99" t="s">
+        <v>45</v>
+      </c>
+      <c r="C12" s="97">
+        <v>200</v>
+      </c>
+      <c r="D12" s="97">
+        <v>152</v>
+      </c>
+      <c r="E12" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="G12" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I12" s="98">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
+      <c r="A13" s="97">
+        <v>50</v>
+      </c>
+      <c r="B13" s="99" t="s">
+        <v>46</v>
+      </c>
+      <c r="C13" s="97">
+        <v>250</v>
+      </c>
+      <c r="D13" s="97">
+        <v>157</v>
+      </c>
+      <c r="E13" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="F13" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="G13" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="H13" s="100" t="s">
+        <v>47</v>
+      </c>
+      <c r="I13" s="98">
+        <v>79</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Končan GUI in s tem projekt (skoraj)
</commit_message>
<xml_diff>
--- a/Meje za meritve.xlsx
+++ b/Meje za meritve.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jasak\ProjektAljaz\Avtomatiziranje-elektro-zapiskov\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F1067D2-6D34-41F1-B8FE-2109CDC08CA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCA9D425-F20E-4036-B0C2-711D3B404005}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-83" yWindow="0" windowWidth="14566" windowHeight="15563" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="28996" windowHeight="15675" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="gG" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
   <si>
     <t>Nazivni tok nadtokovne zaščite</t>
   </si>
@@ -702,16 +702,21 @@
   <si>
     <t>X</t>
   </si>
+  <si>
+    <t>K</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="###0.0;###0.0"/>
+    <numFmt numFmtId="167" formatCode="###0;###0"/>
   </numFmts>
-  <fonts count="21" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -844,8 +849,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -888,8 +906,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="31">
+  <borders count="32">
     <border>
       <left/>
       <right/>
@@ -1285,11 +1309,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1507,6 +1540,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="20" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="22" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="167" fontId="22" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1552,32 +1612,20 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="31" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" shrinkToFit="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="29" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="165" fontId="21" fillId="0" borderId="30" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1585,6 +1633,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFD3D3D3"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1931,24 +1984,24 @@
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="84" t="s">
+      <c r="A1" s="93" t="s">
         <v>19</v>
       </c>
-      <c r="B1" s="84"/>
-      <c r="C1" s="84"/>
-      <c r="D1" s="85" t="s">
+      <c r="B1" s="93"/>
+      <c r="C1" s="93"/>
+      <c r="D1" s="94" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="87" t="s">
+      <c r="E1" s="95"/>
+      <c r="F1" s="95"/>
+      <c r="G1" s="96" t="s">
         <v>21</v>
       </c>
-      <c r="H1" s="87"/>
-      <c r="I1" s="87"/>
-      <c r="J1" s="87"/>
-      <c r="K1" s="87"/>
-      <c r="L1" s="88"/>
+      <c r="H1" s="96"/>
+      <c r="I1" s="96"/>
+      <c r="J1" s="96"/>
+      <c r="K1" s="96"/>
+      <c r="L1" s="97"/>
     </row>
     <row r="2" spans="1:12" ht="51" thickTop="1" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
@@ -2027,26 +2080,26 @@
       </c>
     </row>
     <row r="4" spans="1:12" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="77" t="s">
+      <c r="A4" s="86" t="s">
         <v>22</v>
       </c>
-      <c r="B4" s="78"/>
-      <c r="C4" s="78"/>
-      <c r="D4" s="79" t="s">
+      <c r="B4" s="87"/>
+      <c r="C4" s="87"/>
+      <c r="D4" s="88" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="81" t="s">
+      <c r="E4" s="89"/>
+      <c r="F4" s="89"/>
+      <c r="G4" s="90" t="s">
         <v>23</v>
       </c>
-      <c r="H4" s="82"/>
-      <c r="I4" s="83"/>
-      <c r="J4" s="89" t="s">
+      <c r="H4" s="91"/>
+      <c r="I4" s="92"/>
+      <c r="J4" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="K4" s="90"/>
-      <c r="L4" s="91"/>
+      <c r="K4" s="99"/>
+      <c r="L4" s="100"/>
     </row>
     <row r="5" spans="1:12" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A5" s="11" t="s">
@@ -3244,15 +3297,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45729BEE-1996-442E-89AE-88EE1CAC8D80}">
-  <dimension ref="A1:G20"/>
+  <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="R11" sqref="R11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A1" s="13"/>
       <c r="B1" s="76" t="s">
         <v>10</v>
@@ -3262,12 +3315,16 @@
         <v>11</v>
       </c>
       <c r="E1" s="14"/>
-      <c r="F1" s="92" t="s">
+      <c r="F1" s="103" t="s">
         <v>12</v>
       </c>
-      <c r="G1" s="93"/>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="G1" s="104"/>
+      <c r="H1" s="101" t="s">
+        <v>48</v>
+      </c>
+      <c r="I1" s="102"/>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A2" s="16"/>
       <c r="B2" s="17" t="s">
         <v>13</v>
@@ -3281,8 +3338,10 @@
         <v>15</v>
       </c>
       <c r="G2" s="18"/>
-    </row>
-    <row r="3" spans="1:7" ht="41.65" x14ac:dyDescent="0.45">
+      <c r="H2" s="101"/>
+      <c r="I2" s="102"/>
+    </row>
+    <row r="3" spans="1:9" ht="41.65" customHeight="1" x14ac:dyDescent="0.45">
       <c r="A3" s="20" t="s">
         <v>16</v>
       </c>
@@ -3305,7 +3364,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A4" s="23" t="s">
         <v>8</v>
       </c>
@@ -3327,8 +3386,14 @@
       <c r="G4" s="25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H4" s="24" t="s">
+        <v>8</v>
+      </c>
+      <c r="I4" s="25" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A5" s="26"/>
       <c r="B5" s="27"/>
       <c r="C5" s="27"/>
@@ -3337,7 +3402,7 @@
       <c r="F5" s="27"/>
       <c r="G5" s="27"/>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A6" s="24">
         <v>2</v>
       </c>
@@ -3359,8 +3424,14 @@
       <c r="G6" s="28">
         <v>5.7</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H6" s="105">
+        <v>0.5</v>
+      </c>
+      <c r="I6" s="84">
+        <v>9.4</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A7" s="24">
         <v>4</v>
       </c>
@@ -3382,8 +3453,14 @@
       <c r="G7" s="28">
         <v>2.8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H7" s="105">
+        <v>1</v>
+      </c>
+      <c r="I7" s="84">
+        <v>18.8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A8" s="24">
         <v>6</v>
       </c>
@@ -3405,8 +3482,14 @@
       <c r="G8" s="28">
         <v>1.9</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H8" s="105">
+        <v>1.6</v>
+      </c>
+      <c r="I8" s="85">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9" s="24">
         <v>8</v>
       </c>
@@ -3428,8 +3511,14 @@
       <c r="G9" s="28">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H9" s="105">
+        <v>2</v>
+      </c>
+      <c r="I9" s="84">
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10" s="29">
         <v>10</v>
       </c>
@@ -3451,8 +3540,14 @@
       <c r="G10" s="32">
         <v>1.1000000000000001</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H10" s="105">
+        <v>4</v>
+      </c>
+      <c r="I10" s="85">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11" s="29">
         <v>16</v>
       </c>
@@ -3474,8 +3569,14 @@
       <c r="G11" s="32">
         <v>0.7</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H11" s="105">
+        <v>6</v>
+      </c>
+      <c r="I11" s="84">
+        <v>112.5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12" s="29">
         <v>20</v>
       </c>
@@ -3497,8 +3598,14 @@
       <c r="G12" s="32">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H12" s="105">
+        <v>10</v>
+      </c>
+      <c r="I12" s="84">
+        <v>187.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A13" s="24">
         <v>25</v>
       </c>
@@ -3520,8 +3627,14 @@
       <c r="G13" s="32">
         <v>0.4</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H13" s="105">
+        <v>13</v>
+      </c>
+      <c r="I13" s="84">
+        <v>243.8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14" s="24">
         <v>32</v>
       </c>
@@ -3543,8 +3656,14 @@
       <c r="G14" s="32">
         <v>0.3</v>
       </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H14" s="105">
+        <v>15</v>
+      </c>
+      <c r="I14" s="84">
+        <v>281.3</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15" s="24">
         <v>40</v>
       </c>
@@ -3566,8 +3685,14 @@
       <c r="G15" s="32">
         <v>0.28000000000000003</v>
       </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H15" s="105">
+        <v>16</v>
+      </c>
+      <c r="I15" s="85">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16" s="24">
         <v>50</v>
       </c>
@@ -3589,8 +3714,14 @@
       <c r="G16" s="32">
         <v>0.23</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H16" s="105">
+        <v>20</v>
+      </c>
+      <c r="I16" s="85">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17" s="24">
         <v>63</v>
       </c>
@@ -3612,8 +3743,14 @@
       <c r="G17" s="32">
         <v>0.18</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H17" s="105">
+        <v>25</v>
+      </c>
+      <c r="I17" s="84">
+        <v>468.8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18" s="24"/>
       <c r="B18" s="24"/>
       <c r="C18" s="28"/>
@@ -3621,8 +3758,14 @@
       <c r="E18" s="28"/>
       <c r="F18" s="24"/>
       <c r="G18" s="28"/>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.45">
+      <c r="H18" s="105">
+        <v>32</v>
+      </c>
+      <c r="I18" s="85">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19" s="24"/>
       <c r="B19" s="24"/>
       <c r="C19" s="28"/>
@@ -3631,7 +3774,7 @@
       <c r="F19" s="24"/>
       <c r="G19" s="28"/>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A20" s="24"/>
       <c r="B20" s="24"/>
       <c r="C20" s="28"/>
@@ -3641,10 +3784,12 @@
       <c r="G20" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
+    <mergeCell ref="H1:I2"/>
     <mergeCell ref="F1:G1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3681,11 +3826,11 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" s="89" t="s">
+      <c r="A3" s="98" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="90"/>
-      <c r="C3" s="91"/>
+      <c r="B3" s="99"/>
+      <c r="C3" s="100"/>
     </row>
     <row r="4" spans="1:3" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
       <c r="A4" s="10" t="s">
@@ -4058,386 +4203,386 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3B4FE9D0-D252-4B66-A7CF-69234516F26F}">
   <dimension ref="A1:I13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K3" sqref="K3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <sheetData>
     <row r="1" spans="1:9" ht="106.5" x14ac:dyDescent="0.45">
-      <c r="A1" s="94" t="s">
+      <c r="A1" s="77" t="s">
         <v>28</v>
       </c>
-      <c r="B1" s="94" t="s">
+      <c r="B1" s="77" t="s">
         <v>29</v>
       </c>
-      <c r="C1" s="94" t="s">
+      <c r="C1" s="77" t="s">
         <v>30</v>
       </c>
-      <c r="D1" s="94" t="s">
+      <c r="D1" s="77" t="s">
         <v>31</v>
       </c>
-      <c r="E1" s="94" t="s">
+      <c r="E1" s="77" t="s">
         <v>32</v>
       </c>
-      <c r="F1" s="94" t="s">
+      <c r="F1" s="77" t="s">
         <v>33</v>
       </c>
-      <c r="G1" s="94" t="s">
+      <c r="G1" s="77" t="s">
         <v>34</v>
       </c>
-      <c r="H1" s="94" t="s">
+      <c r="H1" s="77" t="s">
         <v>35</v>
       </c>
-      <c r="I1" s="95" t="s">
+      <c r="I1" s="78" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A2" s="97">
+      <c r="A2" s="80">
         <v>500</v>
       </c>
-      <c r="B2" s="96" t="s">
+      <c r="B2" s="79" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="97">
+      <c r="C2" s="80">
         <v>16</v>
       </c>
-      <c r="D2" s="97">
+      <c r="D2" s="80">
         <v>97</v>
       </c>
-      <c r="E2" s="97">
+      <c r="E2" s="80">
         <v>53</v>
       </c>
-      <c r="F2" s="97">
+      <c r="F2" s="80">
         <v>76</v>
       </c>
-      <c r="G2" s="97">
+      <c r="G2" s="80">
         <v>30</v>
       </c>
-      <c r="H2" s="97">
+      <c r="H2" s="80">
         <v>7</v>
       </c>
-      <c r="I2" s="98">
+      <c r="I2" s="81">
         <v>31</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A3" s="97">
+      <c r="A3" s="80">
         <v>500</v>
       </c>
-      <c r="B3" s="96" t="s">
+      <c r="B3" s="79" t="s">
         <v>38</v>
       </c>
-      <c r="C3" s="97">
+      <c r="C3" s="80">
         <v>20</v>
       </c>
-      <c r="D3" s="97">
+      <c r="D3" s="80">
         <v>115</v>
       </c>
-      <c r="E3" s="97">
+      <c r="E3" s="80">
         <v>57</v>
       </c>
-      <c r="F3" s="97">
+      <c r="F3" s="80">
         <v>94</v>
       </c>
-      <c r="G3" s="97">
+      <c r="G3" s="80">
         <v>34</v>
       </c>
-      <c r="H3" s="97">
+      <c r="H3" s="80">
         <v>3</v>
       </c>
-      <c r="I3" s="98">
+      <c r="I3" s="81">
         <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A4" s="97">
+      <c r="A4" s="80">
         <v>500</v>
       </c>
-      <c r="B4" s="96" t="s">
+      <c r="B4" s="79" t="s">
         <v>39</v>
       </c>
-      <c r="C4" s="97">
+      <c r="C4" s="80">
         <v>25</v>
       </c>
-      <c r="D4" s="97">
+      <c r="D4" s="80">
         <v>135</v>
       </c>
-      <c r="E4" s="97">
+      <c r="E4" s="80">
         <v>66</v>
       </c>
-      <c r="F4" s="97">
+      <c r="F4" s="80">
         <v>114</v>
       </c>
-      <c r="G4" s="97">
+      <c r="G4" s="80">
         <v>35</v>
       </c>
-      <c r="H4" s="100" t="s">
+      <c r="H4" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I4" s="98">
+      <c r="I4" s="81">
         <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A5" s="97">
+      <c r="A5" s="80">
         <v>400</v>
       </c>
-      <c r="B5" s="96" t="s">
+      <c r="B5" s="79" t="s">
         <v>40</v>
       </c>
-      <c r="C5" s="97">
+      <c r="C5" s="80">
         <v>32</v>
       </c>
-      <c r="D5" s="97">
+      <c r="D5" s="80">
         <v>145</v>
       </c>
-      <c r="E5" s="97">
+      <c r="E5" s="80">
         <v>59</v>
       </c>
-      <c r="F5" s="97">
+      <c r="F5" s="80">
         <v>133</v>
       </c>
-      <c r="G5" s="97">
+      <c r="G5" s="80">
         <v>40</v>
       </c>
-      <c r="H5" s="100" t="s">
+      <c r="H5" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I5" s="98">
+      <c r="I5" s="81">
         <v>42</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A6" s="97">
+      <c r="A6" s="80">
         <v>300</v>
       </c>
-      <c r="B6" s="97">
+      <c r="B6" s="80">
         <v>10</v>
       </c>
-      <c r="C6" s="97">
+      <c r="C6" s="80">
         <v>50</v>
       </c>
-      <c r="D6" s="97">
+      <c r="D6" s="80">
         <v>125</v>
       </c>
-      <c r="E6" s="97">
+      <c r="E6" s="80">
         <v>41</v>
       </c>
-      <c r="F6" s="97">
+      <c r="F6" s="80">
         <v>132</v>
       </c>
-      <c r="G6" s="97">
+      <c r="G6" s="80">
         <v>33</v>
       </c>
-      <c r="H6" s="100" t="s">
+      <c r="H6" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I6" s="98">
+      <c r="I6" s="81">
         <v>37</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A7" s="97">
+      <c r="A7" s="80">
         <v>200</v>
       </c>
-      <c r="B7" s="97">
+      <c r="B7" s="80">
         <v>16</v>
       </c>
-      <c r="C7" s="97">
+      <c r="C7" s="80">
         <v>63</v>
       </c>
-      <c r="D7" s="97">
+      <c r="D7" s="80">
         <v>175</v>
       </c>
-      <c r="E7" s="97">
+      <c r="E7" s="80">
         <v>73</v>
       </c>
-      <c r="F7" s="97">
+      <c r="F7" s="80">
         <v>179</v>
       </c>
-      <c r="G7" s="97">
+      <c r="G7" s="80">
         <v>55</v>
       </c>
-      <c r="H7" s="100" t="s">
+      <c r="H7" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I7" s="98">
+      <c r="I7" s="81">
         <v>61</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A8" s="97">
+      <c r="A8" s="80">
         <v>200</v>
       </c>
-      <c r="B8" s="99" t="s">
+      <c r="B8" s="82" t="s">
         <v>41</v>
       </c>
-      <c r="C8" s="97">
+      <c r="C8" s="80">
         <v>80</v>
       </c>
-      <c r="D8" s="97">
+      <c r="D8" s="80">
         <v>133</v>
       </c>
-      <c r="E8" s="100" t="s">
+      <c r="E8" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="100" t="s">
+      <c r="F8" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G8" s="100" t="s">
+      <c r="G8" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="H8" s="100" t="s">
+      <c r="H8" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I8" s="98">
+      <c r="I8" s="81">
         <v>38</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A9" s="97">
+      <c r="A9" s="80">
         <v>100</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="C9" s="97">
+      <c r="C9" s="80">
         <v>100</v>
       </c>
-      <c r="D9" s="97">
+      <c r="D9" s="80">
         <v>136</v>
       </c>
-      <c r="E9" s="100" t="s">
+      <c r="E9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F9" s="100" t="s">
+      <c r="F9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G9" s="100" t="s">
+      <c r="G9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="H9" s="100" t="s">
+      <c r="H9" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I9" s="98">
+      <c r="I9" s="81">
         <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A10" s="97">
+      <c r="A10" s="80">
         <v>100</v>
       </c>
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="82" t="s">
         <v>43</v>
       </c>
-      <c r="C10" s="97">
+      <c r="C10" s="80">
         <v>125</v>
       </c>
-      <c r="D10" s="97">
+      <c r="D10" s="80">
         <v>141</v>
       </c>
-      <c r="E10" s="100" t="s">
+      <c r="E10" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F10" s="100" t="s">
+      <c r="F10" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="100" t="s">
+      <c r="G10" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="H10" s="100" t="s">
+      <c r="H10" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I10" s="98">
+      <c r="I10" s="81">
         <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A11" s="97">
+      <c r="A11" s="80">
         <v>100</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="82" t="s">
         <v>44</v>
       </c>
-      <c r="C11" s="97">
+      <c r="C11" s="80">
         <v>160</v>
       </c>
-      <c r="D11" s="97">
+      <c r="D11" s="80">
         <v>138</v>
       </c>
-      <c r="E11" s="100" t="s">
+      <c r="E11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F11" s="100" t="s">
+      <c r="F11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G11" s="100" t="s">
+      <c r="G11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="H11" s="100" t="s">
+      <c r="H11" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I11" s="98">
+      <c r="I11" s="81">
         <v>46</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A12" s="97">
+      <c r="A12" s="80">
         <v>50</v>
       </c>
-      <c r="B12" s="99" t="s">
+      <c r="B12" s="82" t="s">
         <v>45</v>
       </c>
-      <c r="C12" s="97">
+      <c r="C12" s="80">
         <v>200</v>
       </c>
-      <c r="D12" s="97">
+      <c r="D12" s="80">
         <v>152</v>
       </c>
-      <c r="E12" s="100" t="s">
+      <c r="E12" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F12" s="100" t="s">
+      <c r="F12" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G12" s="100" t="s">
+      <c r="G12" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="H12" s="100" t="s">
+      <c r="H12" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I12" s="98">
+      <c r="I12" s="81">
         <v>98</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.45">
-      <c r="A13" s="97">
+      <c r="A13" s="80">
         <v>50</v>
       </c>
-      <c r="B13" s="99" t="s">
+      <c r="B13" s="82" t="s">
         <v>46</v>
       </c>
-      <c r="C13" s="97">
+      <c r="C13" s="80">
         <v>250</v>
       </c>
-      <c r="D13" s="97">
+      <c r="D13" s="80">
         <v>157</v>
       </c>
-      <c r="E13" s="100" t="s">
+      <c r="E13" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="F13" s="100" t="s">
+      <c r="F13" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="G13" s="100" t="s">
+      <c r="G13" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="H13" s="100" t="s">
+      <c r="H13" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="I13" s="98">
+      <c r="I13" s="81">
         <v>79</v>
       </c>
     </row>

</xml_diff>